<commit_message>
Updating functionalities required by 'cb' parameter
</commit_message>
<xml_diff>
--- a/src_files/data_files/demanddata_other.xlsx
+++ b/src_files/data_files/demanddata_other.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\BB\bb-master\north_european_model\src_files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\BB\bb-master\north_european_model\src_files\data_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3CE2CDE-C780-47BD-8D3F-844D56BDEB5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76B7F3C5-BBB5-4852-81DE-7EF48A018A45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1125" yWindow="1125" windowWidth="21600" windowHeight="12645" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-105" windowWidth="29040" windowHeight="17520" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Readme" sheetId="2" r:id="rId1"/>
@@ -19,7 +19,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'demanddata_other demands'!$A$1:$F$1</definedName>
   </definedNames>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="73">
   <si>
     <t>Scenario</t>
   </si>
@@ -257,6 +257,9 @@
   </si>
   <si>
     <t>Duplicate entries in any of the sheets</t>
+  </si>
+  <si>
+    <t>steam</t>
   </si>
 </sst>
 </file>
@@ -781,8 +784,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G66"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K34" sqref="K34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1249,6 +1252,9 @@
         <v>10</v>
       </c>
       <c r="B27" t="s">
+        <v>72</v>
+      </c>
+      <c r="C27" t="s">
         <v>21</v>
       </c>
       <c r="D27" t="s">
@@ -1266,6 +1272,9 @@
         <v>10</v>
       </c>
       <c r="B28" t="s">
+        <v>72</v>
+      </c>
+      <c r="C28" t="s">
         <v>21</v>
       </c>
       <c r="D28" t="s">
@@ -1283,9 +1292,11 @@
         <v>10</v>
       </c>
       <c r="B29" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C29" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C29" s="4"/>
       <c r="D29" s="4" t="s">
         <v>24</v>
       </c>
@@ -1593,6 +1604,9 @@
         <v>3</v>
       </c>
       <c r="B47" t="s">
+        <v>72</v>
+      </c>
+      <c r="C47" t="s">
         <v>21</v>
       </c>
       <c r="D47" t="s">
@@ -1610,6 +1624,9 @@
         <v>4</v>
       </c>
       <c r="B48" t="s">
+        <v>72</v>
+      </c>
+      <c r="C48" t="s">
         <v>21</v>
       </c>
       <c r="D48" t="s">
@@ -1627,6 +1644,9 @@
         <v>5</v>
       </c>
       <c r="B49" t="s">
+        <v>72</v>
+      </c>
+      <c r="C49" t="s">
         <v>21</v>
       </c>
       <c r="D49" t="s">
@@ -1644,6 +1664,9 @@
         <v>6</v>
       </c>
       <c r="B50" t="s">
+        <v>72</v>
+      </c>
+      <c r="C50" t="s">
         <v>21</v>
       </c>
       <c r="D50" t="s">
@@ -1661,6 +1684,9 @@
         <v>7</v>
       </c>
       <c r="B51" t="s">
+        <v>72</v>
+      </c>
+      <c r="C51" t="s">
         <v>21</v>
       </c>
       <c r="D51" t="s">
@@ -1678,6 +1704,9 @@
         <v>8</v>
       </c>
       <c r="B52" t="s">
+        <v>72</v>
+      </c>
+      <c r="C52" t="s">
         <v>21</v>
       </c>
       <c r="D52" t="s">
@@ -1695,6 +1724,9 @@
         <v>9</v>
       </c>
       <c r="B53" t="s">
+        <v>72</v>
+      </c>
+      <c r="C53" t="s">
         <v>21</v>
       </c>
       <c r="D53" t="s">
@@ -1712,6 +1744,9 @@
         <v>14</v>
       </c>
       <c r="B54" t="s">
+        <v>72</v>
+      </c>
+      <c r="C54" t="s">
         <v>21</v>
       </c>
       <c r="D54" t="s">
@@ -1729,6 +1764,9 @@
         <v>15</v>
       </c>
       <c r="B55" t="s">
+        <v>72</v>
+      </c>
+      <c r="C55" t="s">
         <v>21</v>
       </c>
       <c r="D55" t="s">
@@ -1746,6 +1784,9 @@
         <v>16</v>
       </c>
       <c r="B56" t="s">
+        <v>72</v>
+      </c>
+      <c r="C56" t="s">
         <v>21</v>
       </c>
       <c r="D56" t="s">
@@ -1763,6 +1804,9 @@
         <v>17</v>
       </c>
       <c r="B57" t="s">
+        <v>72</v>
+      </c>
+      <c r="C57" t="s">
         <v>21</v>
       </c>
       <c r="D57" t="s">
@@ -1780,6 +1824,9 @@
         <v>10</v>
       </c>
       <c r="B58" t="s">
+        <v>72</v>
+      </c>
+      <c r="C58" t="s">
         <v>21</v>
       </c>
       <c r="D58" t="s">
@@ -1797,6 +1844,9 @@
         <v>11</v>
       </c>
       <c r="B59" t="s">
+        <v>72</v>
+      </c>
+      <c r="C59" t="s">
         <v>21</v>
       </c>
       <c r="D59" t="s">
@@ -1814,6 +1864,9 @@
         <v>12</v>
       </c>
       <c r="B60" t="s">
+        <v>72</v>
+      </c>
+      <c r="C60" t="s">
         <v>21</v>
       </c>
       <c r="D60" t="s">
@@ -1831,6 +1884,9 @@
         <v>13</v>
       </c>
       <c r="B61" t="s">
+        <v>72</v>
+      </c>
+      <c r="C61" t="s">
         <v>21</v>
       </c>
       <c r="D61" t="s">

</xml_diff>

<commit_message>
DH update for FI, EE, LV, and LT. Limiting hydro power minimum generation to max 30% of capacity. Updating industrial steam demand and generation capacity.
</commit_message>
<xml_diff>
--- a/src_files/data_files/demanddata_other.xlsx
+++ b/src_files/data_files/demanddata_other.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\BB\bb-master\north_european_model\src_files\data_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76B7F3C5-BBB5-4852-81DE-7EF48A018A45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{013D8619-5D33-44DA-BEFB-D3B8044F004A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-105" windowWidth="29040" windowHeight="17520" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Readme" sheetId="2" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="66">
   <si>
     <t>Scenario</t>
   </si>
@@ -57,9 +57,6 @@
     <t>FR00</t>
   </si>
   <si>
-    <t>UK00</t>
-  </si>
-  <si>
     <t>ES00</t>
   </si>
   <si>
@@ -69,21 +66,9 @@
     <t>NL00</t>
   </si>
   <si>
-    <t>BE00</t>
-  </si>
-  <si>
     <t>FI00</t>
   </si>
   <si>
-    <t>LT00</t>
-  </si>
-  <si>
-    <t>LV00</t>
-  </si>
-  <si>
-    <t>EE00</t>
-  </si>
-  <si>
     <t>SE01</t>
   </si>
   <si>
@@ -97,12 +82,6 @@
   </si>
   <si>
     <t>DKW1</t>
-  </si>
-  <si>
-    <t>DKE1</t>
-  </si>
-  <si>
-    <t>H2 heavy</t>
   </si>
   <si>
     <t>industry</t>
@@ -446,8 +425,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{618B6211-7040-488C-9F85-846A32BD1FFB}" name="Table2" displayName="Table2" ref="A1:G61" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="A1:G61" xr:uid="{618B6211-7040-488C-9F85-846A32BD1FFB}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{618B6211-7040-488C-9F85-846A32BD1FFB}" name="Table2" displayName="Table2" ref="A1:G29" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A1:G29" xr:uid="{618B6211-7040-488C-9F85-846A32BD1FFB}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{D52E40C5-11BB-43CE-8C1E-96C938C2BA4F}" name="Country" dataDxfId="3"/>
     <tableColumn id="2" xr3:uid="{B8F62FBD-B0BB-46F4-A396-0D64F902258F}" name="Grid"/>
@@ -589,189 +568,189 @@
   <sheetData>
     <row r="4" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B4" s="15" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B6" s="15" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B7" s="14" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B8" s="14" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B9" s="14" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B11" s="15" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C12" s="14" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="D12" s="14" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C13" s="14" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="D13" s="14" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C14" s="14" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="D14" s="14" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C15" s="14" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="D15" s="14" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C16" s="14" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="D16" s="14" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C17" s="14" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="D17" s="14" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C18" s="14" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="D18" s="14" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B20" s="15" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C21" s="14" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="D21" s="14" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C22" s="14" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="D22" s="14" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B24" s="15" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C26" s="14" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C27" s="14" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C28" s="14" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C29" s="14" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C31" s="14" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C32" s="14" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
     </row>
     <row r="35" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B35" s="15" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
     </row>
     <row r="36" spans="2:3" x14ac:dyDescent="0.2">
       <c r="C36" s="14" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
     </row>
     <row r="37" spans="2:3" x14ac:dyDescent="0.2">
       <c r="C37" s="14" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
     </row>
     <row r="39" spans="2:3" x14ac:dyDescent="0.2">
       <c r="C39" s="14" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
     </row>
     <row r="40" spans="2:3" x14ac:dyDescent="0.2">
       <c r="C40" s="14" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
     </row>
     <row r="42" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B42" s="15" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
     </row>
     <row r="43" spans="2:3" x14ac:dyDescent="0.2">
       <c r="C43" s="14" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
     </row>
     <row r="44" spans="2:3" x14ac:dyDescent="0.2">
       <c r="C44" s="14" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
     </row>
     <row r="45" spans="2:3" x14ac:dyDescent="0.2">
       <c r="C45" s="14" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -782,10 +761,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G66"/>
+  <dimension ref="A1:G34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K34" sqref="K34"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -800,13 +779,13 @@
   <sheetData>
     <row r="1" spans="1:7" ht="15" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>0</v>
@@ -815,22 +794,22 @@
         <v>1</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="G1" s="10" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="E2" s="6">
         <v>2025</v>
@@ -841,13 +820,13 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="E3" s="7">
         <v>2025</v>
@@ -858,13 +837,13 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" t="s">
         <v>15</v>
-      </c>
-      <c r="B4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4" t="s">
-        <v>22</v>
       </c>
       <c r="E4" s="7">
         <v>2025</v>
@@ -875,13 +854,13 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="B5" t="s">
         <v>2</v>
       </c>
       <c r="D5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="E5" s="7">
         <v>2025</v>
@@ -892,13 +871,13 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B6" t="s">
         <v>2</v>
       </c>
       <c r="D6" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="E6" s="7">
         <v>2040</v>
@@ -909,13 +888,13 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B7" t="s">
         <v>2</v>
       </c>
       <c r="D7" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="E7" s="7">
         <v>2040</v>
@@ -926,13 +905,13 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B8" t="s">
         <v>2</v>
       </c>
       <c r="D8" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="E8" s="7">
         <v>2040</v>
@@ -943,13 +922,13 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B9" t="s">
         <v>2</v>
       </c>
       <c r="D9" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="E9" s="7">
         <v>2040</v>
@@ -960,13 +939,13 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="B10" t="s">
         <v>2</v>
       </c>
       <c r="D10" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="E10" s="7">
         <v>2040</v>
@@ -977,13 +956,13 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="B11" t="s">
         <v>2</v>
       </c>
       <c r="D11" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="E11" s="7">
         <v>2040</v>
@@ -994,13 +973,13 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B12" t="s">
         <v>2</v>
       </c>
       <c r="D12" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="E12" s="7">
         <v>2040</v>
@@ -1017,7 +996,7 @@
         <v>2</v>
       </c>
       <c r="D13" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="E13" s="7">
         <v>2025</v>
@@ -1034,7 +1013,7 @@
         <v>2</v>
       </c>
       <c r="D14" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="E14" s="7">
         <v>2040</v>
@@ -1051,7 +1030,7 @@
         <v>2</v>
       </c>
       <c r="D15" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="E15" s="7">
         <v>2040</v>
@@ -1062,13 +1041,13 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B16" t="s">
         <v>2</v>
       </c>
       <c r="D16" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="E16" s="7">
         <v>2040</v>
@@ -1079,13 +1058,13 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B17" t="s">
         <v>2</v>
       </c>
       <c r="D17" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="E17" s="7">
         <v>2040</v>
@@ -1096,13 +1075,13 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="B18" t="s">
         <v>2</v>
       </c>
       <c r="D18" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="E18" s="7">
         <v>2040</v>
@@ -1113,13 +1092,13 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B19" t="s">
         <v>2</v>
       </c>
       <c r="D19" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="E19" s="7">
         <v>2030</v>
@@ -1130,13 +1109,13 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B20" t="s">
         <v>2</v>
       </c>
       <c r="D20" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="E20" s="7">
         <v>2030</v>
@@ -1147,13 +1126,13 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B21" t="s">
         <v>2</v>
       </c>
       <c r="D21" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="E21" s="7">
         <v>2030</v>
@@ -1164,13 +1143,13 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="B22" t="s">
         <v>2</v>
       </c>
       <c r="D22" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="E22" s="7">
         <v>2030</v>
@@ -1187,7 +1166,7 @@
         <v>2</v>
       </c>
       <c r="D23" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="E23" s="7">
         <v>2030</v>
@@ -1204,7 +1183,7 @@
         <v>2</v>
       </c>
       <c r="D24" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="E24" s="7">
         <v>2030</v>
@@ -1215,13 +1194,13 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B25" t="s">
         <v>2</v>
       </c>
       <c r="D25" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="E25" s="7">
         <v>2040</v>
@@ -1232,13 +1211,13 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B26" t="s">
         <v>2</v>
       </c>
       <c r="D26" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="E26" s="7">
         <v>2040</v>
@@ -1249,16 +1228,16 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B27" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="C27" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="D27" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="E27" s="7">
         <v>2025</v>
@@ -1269,16 +1248,16 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B28" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="C28" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="D28" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="E28" s="7">
         <v>2030</v>
@@ -1289,16 +1268,16 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="E29" s="8">
         <v>2040</v>
@@ -1309,610 +1288,19 @@
       <c r="G29" s="5"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>3</v>
-      </c>
-      <c r="B30" t="s">
-        <v>2</v>
-      </c>
-      <c r="D30" t="s">
-        <v>20</v>
-      </c>
-      <c r="E30" s="7">
-        <v>2035</v>
-      </c>
-      <c r="F30" s="11">
-        <v>150.80881990854729</v>
-      </c>
+      <c r="A30" s="2"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>4</v>
-      </c>
-      <c r="B31" t="s">
-        <v>2</v>
-      </c>
-      <c r="D31" t="s">
-        <v>20</v>
-      </c>
-      <c r="E31" s="7">
-        <v>2035</v>
-      </c>
-      <c r="F31" s="11">
-        <v>39.206709461836077</v>
-      </c>
+      <c r="A31" s="2"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>5</v>
-      </c>
-      <c r="B32" t="s">
-        <v>2</v>
-      </c>
-      <c r="D32" t="s">
-        <v>20</v>
-      </c>
-      <c r="E32" s="7">
-        <v>2035</v>
-      </c>
-      <c r="F32" s="11">
-        <v>36.916628561378829</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A33" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B33" t="s">
-        <v>2</v>
-      </c>
-      <c r="D33" t="s">
-        <v>20</v>
-      </c>
-      <c r="E33" s="7">
-        <v>2035</v>
-      </c>
-      <c r="F33" s="11">
-        <v>47.77266092156173</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A34" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B34" t="s">
-        <v>2</v>
-      </c>
-      <c r="D34" t="s">
-        <v>20</v>
-      </c>
-      <c r="E34" s="7">
-        <v>2035</v>
-      </c>
-      <c r="F34" s="11">
-        <v>26.67244987689061</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A35" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B35" t="s">
-        <v>2</v>
-      </c>
-      <c r="D35" t="s">
-        <v>20</v>
-      </c>
-      <c r="E35" s="7">
-        <v>2035</v>
-      </c>
-      <c r="F35" s="11">
-        <v>35.024252550123109</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A36" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B36" t="s">
-        <v>2</v>
-      </c>
-      <c r="D36" t="s">
-        <v>20</v>
-      </c>
-      <c r="E36" s="7">
-        <v>2035</v>
-      </c>
-      <c r="F36" s="11">
-        <v>21.209470629616607</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A37" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B37" t="s">
-        <v>2</v>
-      </c>
-      <c r="D37" t="s">
-        <v>20</v>
-      </c>
-      <c r="E37" s="7">
-        <v>2035</v>
-      </c>
-      <c r="F37" s="11">
-        <v>0.98366170208288384</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A38" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B38" t="s">
-        <v>2</v>
-      </c>
-      <c r="D38" t="s">
-        <v>20</v>
-      </c>
-      <c r="E38" s="7">
-        <v>2035</v>
-      </c>
-      <c r="F38" s="11">
-        <v>1.6482613239997683</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A39" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B39" t="s">
-        <v>2</v>
-      </c>
-      <c r="D39" t="s">
-        <v>20</v>
-      </c>
-      <c r="E39" s="7">
-        <v>2035</v>
-      </c>
-      <c r="F39" s="11">
-        <v>8.6625545388038798</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A40" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B40" t="s">
-        <v>2</v>
-      </c>
-      <c r="D40" t="s">
-        <v>20</v>
-      </c>
-      <c r="E40" s="7">
-        <v>2035</v>
-      </c>
-      <c r="F40" s="11">
-        <v>2.4154151540723134</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A41" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B41" t="s">
-        <v>2</v>
-      </c>
-      <c r="D41" t="s">
-        <v>20</v>
-      </c>
-      <c r="E41" s="7">
-        <v>2035</v>
-      </c>
-      <c r="F41" s="11">
-        <v>5.9499053555429544</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A42" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B42" t="s">
-        <v>2</v>
-      </c>
-      <c r="D42" t="s">
-        <v>20</v>
-      </c>
-      <c r="E42" s="7">
-        <v>2035</v>
-      </c>
-      <c r="F42" s="11">
-        <v>3.9271611235284496</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A43" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B43" t="s">
-        <v>2</v>
-      </c>
-      <c r="D43" t="s">
-        <v>20</v>
-      </c>
-      <c r="E43" s="7">
-        <v>2035</v>
-      </c>
-      <c r="F43" s="11">
-        <v>10.467068237776999</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A44" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B44" t="s">
-        <v>2</v>
-      </c>
-      <c r="D44" t="s">
-        <v>20</v>
-      </c>
-      <c r="E44" s="7">
-        <v>2035</v>
-      </c>
-      <c r="F44" s="11">
-        <v>3.9508265916285619</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A45" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B45" t="s">
-        <v>2</v>
-      </c>
-      <c r="D45" t="s">
-        <v>20</v>
-      </c>
-      <c r="E45" s="7">
-        <v>2035</v>
-      </c>
-      <c r="F45" s="11">
-        <v>1.1362996834329935</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A46" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B46" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C46" s="4"/>
-      <c r="D46" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E46" s="8">
-        <v>2035</v>
-      </c>
-      <c r="F46" s="12">
-        <v>0.84785437917692585</v>
-      </c>
-      <c r="G46" s="5"/>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
-        <v>3</v>
-      </c>
-      <c r="B47" t="s">
-        <v>72</v>
-      </c>
-      <c r="C47" t="s">
-        <v>21</v>
-      </c>
-      <c r="D47" t="s">
-        <v>20</v>
-      </c>
-      <c r="E47" s="7">
-        <v>2035</v>
-      </c>
-      <c r="F47" s="11">
-        <v>89.390575686813193</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
-        <v>4</v>
-      </c>
-      <c r="B48" t="s">
-        <v>72</v>
-      </c>
-      <c r="C48" t="s">
-        <v>21</v>
-      </c>
-      <c r="D48" t="s">
-        <v>20</v>
-      </c>
-      <c r="E48" s="7">
-        <v>2035</v>
-      </c>
-      <c r="F48" s="11">
-        <v>27.497577829670334</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
-        <v>5</v>
-      </c>
-      <c r="B49" t="s">
-        <v>72</v>
-      </c>
-      <c r="C49" t="s">
-        <v>21</v>
-      </c>
-      <c r="D49" t="s">
-        <v>20</v>
-      </c>
-      <c r="E49" s="7">
-        <v>2035</v>
-      </c>
-      <c r="F49" s="11">
-        <v>147.36625717032965</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A50" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B50" t="s">
-        <v>72</v>
-      </c>
-      <c r="C50" t="s">
-        <v>21</v>
-      </c>
-      <c r="D50" t="s">
-        <v>20</v>
-      </c>
-      <c r="E50" s="7">
-        <v>2035</v>
-      </c>
-      <c r="F50" s="11">
-        <v>15.367019423076922</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A51" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B51" t="s">
-        <v>72</v>
-      </c>
-      <c r="C51" t="s">
-        <v>21</v>
-      </c>
-      <c r="D51" t="s">
-        <v>20</v>
-      </c>
-      <c r="E51" s="7">
-        <v>2035</v>
-      </c>
-      <c r="F51" s="11">
-        <v>25.172503763736266</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A52" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B52" t="s">
-        <v>72</v>
-      </c>
-      <c r="C52" t="s">
-        <v>21</v>
-      </c>
-      <c r="D52" t="s">
-        <v>20</v>
-      </c>
-      <c r="E52" s="7">
-        <v>2035</v>
-      </c>
-      <c r="F52" s="11">
-        <v>12.092048901098902</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A53" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B53" t="s">
-        <v>72</v>
-      </c>
-      <c r="C53" t="s">
-        <v>21</v>
-      </c>
-      <c r="D53" t="s">
-        <v>20</v>
-      </c>
-      <c r="E53" s="7">
-        <v>2035</v>
-      </c>
-      <c r="F53" s="11">
-        <v>9.4712947527472533</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A54" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B54" t="s">
-        <v>72</v>
-      </c>
-      <c r="C54" t="s">
-        <v>21</v>
-      </c>
-      <c r="D54" t="s">
-        <v>20</v>
-      </c>
-      <c r="E54" s="7">
-        <v>2035</v>
-      </c>
-      <c r="F54" s="11">
-        <v>1.1403121428571428</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A55" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B55" t="s">
-        <v>72</v>
-      </c>
-      <c r="C55" t="s">
-        <v>21</v>
-      </c>
-      <c r="D55" t="s">
-        <v>20</v>
-      </c>
-      <c r="E55" s="7">
-        <v>2035</v>
-      </c>
-      <c r="F55" s="11">
-        <v>5.0979269230769226</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A56" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B56" t="s">
-        <v>72</v>
-      </c>
-      <c r="C56" t="s">
-        <v>21</v>
-      </c>
-      <c r="D56" t="s">
-        <v>20</v>
-      </c>
-      <c r="E56" s="7">
-        <v>2035</v>
-      </c>
-      <c r="F56" s="11">
-        <v>22.884912390109889</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A57" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B57" t="s">
-        <v>72</v>
-      </c>
-      <c r="C57" t="s">
-        <v>21</v>
-      </c>
-      <c r="D57" t="s">
-        <v>20</v>
-      </c>
-      <c r="E57" s="7">
-        <v>2035</v>
-      </c>
-      <c r="F57" s="11">
-        <v>5.2148953846153843</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A58" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B58" t="s">
-        <v>72</v>
-      </c>
-      <c r="C58" t="s">
-        <v>21</v>
-      </c>
-      <c r="D58" t="s">
-        <v>20</v>
-      </c>
-      <c r="E58" s="7">
-        <v>2035</v>
-      </c>
-      <c r="F58" s="11">
-        <v>20.740078131868131</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A59" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B59" t="s">
-        <v>72</v>
-      </c>
-      <c r="C59" t="s">
-        <v>21</v>
-      </c>
-      <c r="D59" t="s">
-        <v>20</v>
-      </c>
-      <c r="E59" s="7">
-        <v>2035</v>
-      </c>
-      <c r="F59" s="11">
-        <v>3.9464943131868133</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A60" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B60" t="s">
-        <v>72</v>
-      </c>
-      <c r="C60" t="s">
-        <v>21</v>
-      </c>
-      <c r="D60" t="s">
-        <v>20</v>
-      </c>
-      <c r="E60" s="7">
-        <v>2035</v>
-      </c>
-      <c r="F60" s="11">
-        <v>2.2425600000000001</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A61" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B61" t="s">
-        <v>72</v>
-      </c>
-      <c r="C61" t="s">
-        <v>21</v>
-      </c>
-      <c r="D61" t="s">
-        <v>20</v>
-      </c>
-      <c r="E61" s="7">
-        <v>2035</v>
-      </c>
-      <c r="F61" s="11">
-        <v>1.5351418681318683</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A62" s="2"/>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A63" s="2"/>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A64" s="2"/>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A65" s="2"/>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A66" s="2"/>
+      <c r="A32" s="2"/>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A33" s="2"/>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A34" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>